<commit_message>
Profile for other uses added
</commit_message>
<xml_diff>
--- a/Position_surname.xlsx
+++ b/Position_surname.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Werk\220\2025\Project\D3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\IMY220-D1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5ED2E2E-490F-4588-AB0E-1BDA29B3BA66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5117813F-6151-4801-A259-952959ECF976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="149">
   <si>
     <t xml:space="preserve">Position_Surname: </t>
   </si>
@@ -57,6 +57,7 @@
         <sz val="9"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Please change the cell colour to black in the </t>
     </r>
@@ -67,6 +68,7 @@
         <sz val="9"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>Yes/No</t>
     </r>
@@ -76,6 +78,7 @@
         <sz val="9"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> column into the thick border boxes</t>
     </r>
@@ -87,6 +90,7 @@
         <sz val="9"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">If you filled in any of the boxes, you will have to </t>
     </r>
@@ -97,6 +101,7 @@
         <sz val="9"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">show </t>
     </r>
@@ -106,6 +111,7 @@
         <sz val="9"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">and </t>
     </r>
@@ -116,6 +122,7 @@
         <sz val="9"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">explain </t>
     </r>
@@ -125,6 +132,7 @@
         <sz val="9"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>what you did and how you did it</t>
     </r>
@@ -136,6 +144,7 @@
         <sz val="9"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">The project will be marked by interacting with the website </t>
     </r>
@@ -146,6 +155,7 @@
         <sz val="9"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>only</t>
     </r>
@@ -155,6 +165,7 @@
         <sz val="9"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>, except in the "technologies and techniques" section</t>
     </r>
@@ -270,6 +281,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">All the user's </t>
     </r>
@@ -278,6 +290,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>created projects</t>
     </r>
@@ -286,6 +299,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> appear on their profile page</t>
     </r>
@@ -296,6 +310,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">All the user's </t>
     </r>
@@ -304,6 +319,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">saved </t>
     </r>
@@ -312,6 +328,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>projects appear on their profile page</t>
     </r>
@@ -335,6 +352,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">A </t>
     </r>
@@ -345,6 +363,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">registered </t>
     </r>
@@ -354,6 +373,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>user can do the following:</t>
     </r>
@@ -436,6 +456,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Caters for created date (should add </t>
     </r>
@@ -444,6 +465,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">automatically </t>
     </r>
@@ -452,6 +474,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
+        <family val="2"/>
       </rPr>
       <t>and not entered in manually)</t>
     </r>
@@ -683,6 +706,9 @@
   </si>
   <si>
     <t>Total with bonus</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -700,34 +726,40 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -735,6 +767,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -742,6 +775,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -750,6 +784,7 @@
       <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -757,6 +792,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1218,18 +1254,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="110.33203125" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="110.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" customWidth="1"/>
+    <col min="3" max="3" width="8.7109375" customWidth="1"/>
     <col min="4" max="4" width="78" customWidth="1"/>
-    <col min="5" max="26" width="8.6640625" customWidth="1"/>
+    <col min="5" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
@@ -1237,221 +1275,229 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="36" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="36"/>
     </row>
-    <row r="16" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B16" s="36"/>
     </row>
-    <row r="17" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B17" s="36"/>
     </row>
-    <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="36"/>
     </row>
-    <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="36"/>
     </row>
-    <row r="20" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="21" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B22" s="36"/>
     </row>
-    <row r="23" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B23" s="36"/>
     </row>
-    <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B24" s="36"/>
     </row>
-    <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B25" s="36"/>
     </row>
-    <row r="26" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B26" s="36"/>
     </row>
-    <row r="27" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B27" s="36"/>
     </row>
-    <row r="28" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B30" s="8"/>
     </row>
-    <row r="31" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>26</v>
       </c>
       <c r="B31" s="8"/>
     </row>
-    <row r="32" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B32" s="8"/>
     </row>
-    <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="7"/>
     </row>
-    <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="str">
         <f>A1</f>
         <v xml:space="preserve">Position_Surname: </v>
       </c>
       <c r="B34" s="7"/>
     </row>
-    <row r="35" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
     </row>
-    <row r="36" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B38" s="36"/>
+      <c r="B38" s="36" t="s">
+        <v>148</v>
+      </c>
       <c r="C38" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="36"/>
+      <c r="B39" s="36" t="s">
+        <v>148</v>
+      </c>
       <c r="C39" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B40" s="36"/>
+      <c r="B40" s="36" t="s">
+        <v>148</v>
+      </c>
       <c r="C40" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B41" s="36"/>
+      <c r="B41" s="36" t="s">
+        <v>148</v>
+      </c>
       <c r="C41" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
       <c r="B42" s="11"/>
       <c r="C42" s="7"/>
     </row>
-    <row r="43" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
         <v>34</v>
       </c>
@@ -1460,85 +1506,101 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B46" s="36"/>
+      <c r="B46" s="36" t="s">
+        <v>148</v>
+      </c>
       <c r="C46" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B47" s="36"/>
+      <c r="B47" s="36" t="s">
+        <v>148</v>
+      </c>
       <c r="C47" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B48" s="36"/>
+      <c r="B48" s="36" t="s">
+        <v>148</v>
+      </c>
       <c r="C48" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B49" s="36"/>
+      <c r="B49" s="36" t="s">
+        <v>148</v>
+      </c>
       <c r="C49" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B50" s="36"/>
+      <c r="B50" s="36" t="s">
+        <v>148</v>
+      </c>
       <c r="C50" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B51" s="36"/>
+      <c r="B51" s="36" t="s">
+        <v>148</v>
+      </c>
       <c r="C51" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B52" s="36"/>
+      <c r="B52" s="36" t="s">
+        <v>148</v>
+      </c>
       <c r="C52" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B53" s="36"/>
+      <c r="B53" s="36" t="s">
+        <v>148</v>
+      </c>
       <c r="C53" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>44</v>
       </c>
@@ -1547,21 +1609,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="12"/>
       <c r="B55" s="11"/>
       <c r="C55" s="7"/>
     </row>
-    <row r="56" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B56" s="36"/>
+      <c r="B56" s="36" t="s">
+        <v>148</v>
+      </c>
       <c r="C56" s="13">
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
         <v>46</v>
       </c>
@@ -1570,18 +1634,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="59" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>49</v>
       </c>
@@ -1590,7 +1654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>50</v>
       </c>
@@ -1599,7 +1663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
         <v>51</v>
       </c>
@@ -1608,7 +1672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>52</v>
       </c>
@@ -1617,7 +1681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>53</v>
       </c>
@@ -1626,7 +1690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>54</v>
       </c>
@@ -1635,15 +1699,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="11"/>
     </row>
-    <row r="68" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
         <v>56</v>
       </c>
@@ -1652,7 +1716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
         <v>57</v>
       </c>
@@ -1661,7 +1725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
         <v>58</v>
       </c>
@@ -1670,7 +1734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
         <v>59</v>
       </c>
@@ -1679,7 +1743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
         <v>60</v>
       </c>
@@ -1688,7 +1752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
         <v>61</v>
       </c>
@@ -1697,13 +1761,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="76" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
         <v>63</v>
       </c>
@@ -1712,7 +1776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
         <v>64</v>
       </c>
@@ -1721,7 +1785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
         <v>65</v>
       </c>
@@ -1730,7 +1794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
         <v>66</v>
       </c>
@@ -1739,12 +1803,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="12"/>
       <c r="B81" s="11"/>
       <c r="C81" s="7"/>
     </row>
-    <row r="82" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="12" t="s">
         <v>67</v>
       </c>
@@ -1753,7 +1817,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="12" t="s">
         <v>68</v>
       </c>
@@ -1762,7 +1826,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="12" t="s">
         <v>69</v>
       </c>
@@ -1771,17 +1835,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="10"/>
       <c r="B85" s="11"/>
       <c r="C85" s="7"/>
     </row>
-    <row r="86" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="87" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
         <v>71</v>
       </c>
@@ -1790,7 +1854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
         <v>72</v>
       </c>
@@ -1799,7 +1863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
         <v>73</v>
       </c>
@@ -1808,7 +1872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
         <v>74</v>
       </c>
@@ -1817,7 +1881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
         <v>75</v>
       </c>
@@ -1826,12 +1890,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="12"/>
       <c r="B92" s="11"/>
       <c r="C92" s="6"/>
     </row>
-    <row r="93" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="12" t="s">
         <v>76</v>
       </c>
@@ -1840,7 +1904,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="12" t="s">
         <v>77</v>
       </c>
@@ -1849,17 +1913,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="11"/>
       <c r="B95" s="11"/>
       <c r="C95" s="7"/>
     </row>
-    <row r="96" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="14" t="s">
         <v>79</v>
       </c>
@@ -1868,7 +1932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="14" t="s">
         <v>80</v>
       </c>
@@ -1877,7 +1941,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="14" t="s">
         <v>81</v>
       </c>
@@ -1886,7 +1950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
         <v>82</v>
       </c>
@@ -1895,7 +1959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
         <v>83</v>
       </c>
@@ -1904,18 +1968,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B102" s="11"/>
       <c r="C102" s="7"/>
     </row>
-    <row r="103" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="15" t="s">
         <v>84</v>
       </c>
       <c r="B103" s="11"/>
       <c r="C103" s="7"/>
     </row>
-    <row r="104" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="14" t="s">
         <v>85</v>
       </c>
@@ -1924,7 +1988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="14" t="s">
         <v>86</v>
       </c>
@@ -1933,7 +1997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
         <v>87</v>
       </c>
@@ -1942,12 +2006,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="16"/>
       <c r="B107" s="11"/>
       <c r="C107" s="6"/>
     </row>
-    <row r="108" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="16" t="s">
         <v>88</v>
       </c>
@@ -1956,18 +2020,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B109" s="11"/>
       <c r="C109" s="6"/>
     </row>
-    <row r="110" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="15" t="s">
         <v>89</v>
       </c>
       <c r="B110" s="11"/>
       <c r="C110" s="7"/>
     </row>
-    <row r="111" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
         <v>90</v>
       </c>
@@ -1976,7 +2040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="14" t="s">
         <v>91</v>
       </c>
@@ -1985,7 +2049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="14" t="s">
         <v>92</v>
       </c>
@@ -1994,12 +2058,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="14"/>
       <c r="B114" s="11"/>
       <c r="C114" s="6"/>
     </row>
-    <row r="115" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="16" t="s">
         <v>93</v>
       </c>
@@ -2008,7 +2072,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="16" t="s">
         <v>94</v>
       </c>
@@ -2017,26 +2081,26 @@
         <v>2</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A117" s="7"/>
       <c r="B117" s="11"/>
       <c r="C117" s="17"/>
     </row>
-    <row r="118" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
         <v>95</v>
       </c>
       <c r="B118" s="7"/>
       <c r="C118" s="7"/>
     </row>
-    <row r="119" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="7" t="s">
         <v>96</v>
       </c>
       <c r="B119" s="11"/>
       <c r="C119" s="7"/>
     </row>
-    <row r="120" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="6" t="s">
         <v>97</v>
       </c>
@@ -2045,7 +2109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="6" t="s">
         <v>98</v>
       </c>
@@ -2054,7 +2118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="6" t="s">
         <v>99</v>
       </c>
@@ -2063,7 +2127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="s">
         <v>100</v>
       </c>
@@ -2072,7 +2136,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
         <v>101</v>
       </c>
@@ -2081,12 +2145,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="12"/>
       <c r="B125" s="11"/>
       <c r="C125" s="6"/>
     </row>
-    <row r="126" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="12" t="s">
         <v>102</v>
       </c>
@@ -2095,7 +2159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B127" s="11"/>
       <c r="C127" s="7"/>
       <c r="D127" s="7"/>
@@ -2103,7 +2167,7 @@
       <c r="F127" s="7"/>
       <c r="G127" s="7"/>
     </row>
-    <row r="128" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="10" t="s">
         <v>103</v>
       </c>
@@ -2114,7 +2178,7 @@
       <c r="F128" s="7"/>
       <c r="G128" s="7"/>
     </row>
-    <row r="129" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
         <v>104</v>
       </c>
@@ -2125,7 +2189,7 @@
       <c r="F129" s="7"/>
       <c r="G129" s="7"/>
     </row>
-    <row r="130" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="18"/>
       <c r="B130" s="17"/>
       <c r="C130" s="7"/>
@@ -2134,7 +2198,7 @@
       <c r="F130" s="7"/>
       <c r="G130" s="7"/>
     </row>
-    <row r="131" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="19"/>
       <c r="B131" s="20"/>
       <c r="C131" s="7"/>
@@ -2143,7 +2207,7 @@
       <c r="F131" s="7"/>
       <c r="G131" s="7"/>
     </row>
-    <row r="132" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A132" s="19"/>
       <c r="B132" s="20"/>
       <c r="C132" s="7"/>
@@ -2152,7 +2216,7 @@
       <c r="F132" s="7"/>
       <c r="G132" s="7"/>
     </row>
-    <row r="133" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A133" s="21"/>
       <c r="B133" s="22"/>
       <c r="C133" s="7"/>
@@ -2161,7 +2225,7 @@
       <c r="F133" s="7"/>
       <c r="G133" s="7"/>
     </row>
-    <row r="134" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A134" s="10"/>
       <c r="B134" s="7"/>
       <c r="C134" s="7"/>
@@ -2170,7 +2234,7 @@
       <c r="F134" s="7"/>
       <c r="G134" s="7"/>
     </row>
-    <row r="135" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="str">
         <f>A1</f>
         <v xml:space="preserve">Position_Surname: </v>
@@ -2182,25 +2246,25 @@
       <c r="F135" s="7"/>
       <c r="G135" s="7"/>
     </row>
-    <row r="136" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="6" t="s">
         <v>105</v>
       </c>
       <c r="B136" s="8"/>
       <c r="C136" s="9"/>
     </row>
-    <row r="137" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B137" s="7"/>
       <c r="C137" s="7"/>
     </row>
-    <row r="138" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
         <v>106</v>
       </c>
       <c r="B138" s="7"/>
       <c r="C138" s="7"/>
     </row>
-    <row r="139" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="7" t="s">
         <v>107</v>
       </c>
@@ -2209,7 +2273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="7" t="s">
         <v>108</v>
       </c>
@@ -2218,7 +2282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A141" s="23" t="s">
         <v>109</v>
       </c>
@@ -2250,19 +2314,19 @@
       <c r="Y141" s="25"/>
       <c r="Z141" s="25"/>
     </row>
-    <row r="142" spans="1:26" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:26" ht="135" x14ac:dyDescent="0.25">
       <c r="A142" s="26" t="s">
         <v>110</v>
       </c>
       <c r="B142" s="11"/>
       <c r="C142" s="7"/>
     </row>
-    <row r="143" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="12"/>
       <c r="B143" s="11"/>
       <c r="C143" s="7"/>
     </row>
-    <row r="144" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="12" t="s">
         <v>111</v>
       </c>
@@ -2271,18 +2335,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B145" s="7"/>
       <c r="C145" s="7"/>
     </row>
-    <row r="146" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
         <v>112</v>
       </c>
       <c r="B146" s="11"/>
       <c r="C146" s="7"/>
     </row>
-    <row r="147" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="7" t="s">
         <v>113</v>
       </c>
@@ -2291,7 +2355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="6" t="s">
         <v>114</v>
       </c>
@@ -2300,7 +2364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="7" t="s">
         <v>115</v>
       </c>
@@ -2309,7 +2373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="6" t="s">
         <v>116</v>
       </c>
@@ -2318,7 +2382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="6" t="s">
         <v>117</v>
       </c>
@@ -2327,7 +2391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="7" t="s">
         <v>118</v>
       </c>
@@ -2336,7 +2400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="7" t="s">
         <v>119</v>
       </c>
@@ -2345,7 +2409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="6" t="s">
         <v>120</v>
       </c>
@@ -2354,7 +2418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="6" t="s">
         <v>121</v>
       </c>
@@ -2363,7 +2427,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="27" t="s">
         <v>122</v>
       </c>
@@ -2372,7 +2436,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="28" t="s">
         <v>123</v>
       </c>
@@ -2381,12 +2445,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="29"/>
       <c r="B158" s="11"/>
       <c r="C158" s="7"/>
     </row>
-    <row r="159" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="28" t="s">
         <v>124</v>
       </c>
@@ -2395,18 +2459,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="160" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B160" s="7"/>
       <c r="C160" s="7"/>
     </row>
-    <row r="161" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
         <v>125</v>
       </c>
       <c r="B161" s="7"/>
       <c r="C161" s="7"/>
     </row>
-    <row r="162" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="7" t="s">
         <v>126</v>
       </c>
@@ -2415,18 +2479,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="163" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B163" s="7"/>
       <c r="C163" s="7"/>
     </row>
-    <row r="164" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
         <v>127</v>
       </c>
       <c r="B164" s="7"/>
       <c r="C164" s="7"/>
     </row>
-    <row r="165" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="7" t="s">
         <v>128</v>
       </c>
@@ -2435,7 +2499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="7" t="s">
         <v>129</v>
       </c>
@@ -2444,7 +2508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="7" t="s">
         <v>130</v>
       </c>
@@ -2453,7 +2517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="7" t="s">
         <v>131</v>
       </c>
@@ -2462,7 +2526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="7" t="s">
         <v>132</v>
       </c>
@@ -2471,18 +2535,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B170" s="7"/>
       <c r="C170" s="7"/>
     </row>
-    <row r="171" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
         <v>133</v>
       </c>
       <c r="B171" s="7"/>
       <c r="C171" s="7"/>
     </row>
-    <row r="172" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="7" t="s">
         <v>134</v>
       </c>
@@ -2491,7 +2555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="7" t="s">
         <v>135</v>
       </c>
@@ -2500,7 +2564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="7" t="s">
         <v>136</v>
       </c>
@@ -2510,7 +2574,7 @@
       </c>
       <c r="D174" s="7"/>
     </row>
-    <row r="175" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="7" t="s">
         <v>137</v>
       </c>
@@ -2520,7 +2584,7 @@
       </c>
       <c r="D175" s="7"/>
     </row>
-    <row r="176" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="6" t="s">
         <v>138</v>
       </c>
@@ -2530,7 +2594,7 @@
       </c>
       <c r="D176" s="7"/>
     </row>
-    <row r="177" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="6" t="s">
         <v>139</v>
       </c>
@@ -2539,7 +2603,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="178" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="6" t="s">
         <v>140</v>
       </c>
@@ -2548,7 +2612,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="179" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="6" t="s">
         <v>141</v>
       </c>
@@ -2557,7 +2621,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="180" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="6" t="s">
         <v>142</v>
       </c>
@@ -2566,7 +2630,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="181" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="6" t="s">
         <v>143</v>
       </c>
@@ -2575,16 +2639,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="182" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C182" s="7"/>
     </row>
-    <row r="183" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="5" t="s">
         <v>144</v>
       </c>
       <c r="C183" s="7"/>
     </row>
-    <row r="184" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="7" t="s">
         <v>145</v>
       </c>
@@ -2593,43 +2657,43 @@
         <v>2</v>
       </c>
     </row>
-    <row r="185" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C185" s="17"/>
     </row>
-    <row r="186" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="10" t="s">
         <v>103</v>
       </c>
       <c r="B186" s="8"/>
       <c r="C186" s="9"/>
     </row>
-    <row r="187" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="5" t="s">
         <v>104</v>
       </c>
       <c r="C187" s="7"/>
     </row>
-    <row r="188" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="18"/>
       <c r="B188" s="31"/>
       <c r="C188" s="17"/>
     </row>
-    <row r="189" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="19"/>
       <c r="B189" s="7"/>
       <c r="C189" s="20"/>
     </row>
-    <row r="190" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="19"/>
       <c r="B190" s="7"/>
       <c r="C190" s="20"/>
     </row>
-    <row r="191" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="21"/>
       <c r="B191" s="32"/>
       <c r="C191" s="22"/>
     </row>
-    <row r="192" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="33" t="s">
         <v>27</v>
       </c>
@@ -2639,7 +2703,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="193" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="35" t="s">
         <v>146</v>
       </c>
@@ -2649,7 +2713,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="194" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="33" t="s">
         <v>147</v>
       </c>
@@ -2659,813 +2723,813 @@
         <v>137</v>
       </c>
     </row>
-    <row r="195" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="196" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="197" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="198" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="199" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="200" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="201" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="202" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="203" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="204" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="205" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="206" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="207" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="208" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="209" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="210" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="211" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="212" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="213" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="214" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="215" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="216" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="217" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="218" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="219" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="220" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="221" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="222" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="223" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="224" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="225" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="226" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="227" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="228" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="229" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="230" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="231" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="232" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="233" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="234" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="235" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="236" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="237" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="238" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="239" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="240" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="241" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="242" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="243" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="244" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="245" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="246" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="247" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="248" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="249" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="250" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="251" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="252" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="253" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="254" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="255" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="256" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="257" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="258" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="259" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="260" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="261" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="262" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="263" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="264" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="265" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="266" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="267" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="268" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="269" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="270" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="271" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="272" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="273" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="274" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="275" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="276" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="277" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="278" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="279" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="280" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="281" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="282" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="283" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="284" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="285" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="286" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="287" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="288" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="289" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="290" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="291" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="292" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="293" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="294" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="295" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="296" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="297" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="298" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="299" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="300" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="301" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="302" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="303" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="304" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="305" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="306" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="307" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="308" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="309" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="310" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="311" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="312" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="313" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="314" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="315" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="316" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="317" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="318" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="319" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="320" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="321" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="322" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="323" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="324" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="325" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="326" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="327" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="328" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="329" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="330" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="331" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="332" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="333" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="334" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="335" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="336" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="337" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="338" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="339" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="340" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="341" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="342" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="343" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="344" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="345" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="346" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="347" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="348" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="349" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="350" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="351" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="352" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="353" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="354" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="355" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="356" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="357" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="358" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="359" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="360" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="361" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="362" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="363" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="364" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="365" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="366" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="367" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="368" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="369" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="370" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="371" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="372" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="373" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="374" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="375" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="376" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="377" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="378" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="379" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="380" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="381" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="382" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="383" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="384" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="385" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="386" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="387" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="388" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="389" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="390" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="391" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="392" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="393" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="394" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="395" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="396" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="397" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="398" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="399" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="400" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="401" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="402" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="403" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="404" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="405" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="406" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="407" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="408" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="409" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="410" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="411" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="412" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="413" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="414" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="415" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="416" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="417" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="418" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="419" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="420" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="421" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="422" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="423" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="424" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="425" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="426" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="427" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="428" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="429" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="430" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="431" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="432" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="433" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="434" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="435" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="436" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="437" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="438" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="439" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="440" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="441" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="442" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="443" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="444" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="445" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="446" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="447" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="448" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="449" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="450" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="451" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="452" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="453" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="454" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="455" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="456" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="457" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="458" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="459" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="460" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="461" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="462" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="463" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="464" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="465" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="466" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="467" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="468" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="469" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="470" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="471" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="472" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="473" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="474" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="475" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="476" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="477" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="478" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="479" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="480" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="481" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="482" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="483" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="484" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="485" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="486" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="487" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="488" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="489" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="490" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="491" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="492" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="493" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="494" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="495" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="496" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="497" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="498" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="499" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="500" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="501" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="502" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="503" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="504" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="505" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="506" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="507" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="508" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="509" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="510" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="511" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="512" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="513" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="514" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="515" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="516" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="517" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="518" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="519" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="520" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="521" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="522" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="523" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="524" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="525" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="526" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="527" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="528" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="529" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="530" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="531" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="532" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="533" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="534" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="535" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="536" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="537" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="538" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="539" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="540" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="541" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="542" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="543" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="544" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="545" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="546" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="547" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="548" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="549" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="550" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="551" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="552" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="553" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="554" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="555" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="556" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="557" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="558" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="559" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="560" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="561" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="562" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="563" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="564" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="565" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="566" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="567" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="568" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="569" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="570" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="571" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="572" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="573" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="574" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="575" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="576" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="577" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="578" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="579" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="580" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="581" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="582" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="583" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="584" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="585" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="586" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="587" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="588" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="589" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="590" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="591" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="592" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="593" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="594" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="595" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="596" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="597" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="598" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="599" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="600" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="601" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="602" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="603" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="604" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="605" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="606" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="607" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="608" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="609" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="610" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="611" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="612" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="613" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="614" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="615" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="616" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="617" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="618" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="619" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="620" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="621" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="622" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="623" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="624" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="625" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="626" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="627" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="628" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="629" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="630" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="631" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="632" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="633" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="634" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="635" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="636" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="637" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="638" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="639" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="640" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="641" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="642" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="643" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="644" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="645" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="646" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="647" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="648" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="649" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="650" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="651" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="652" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="653" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="654" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="655" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="656" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="657" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="658" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="659" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="660" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="661" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="662" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="663" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="664" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="665" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="666" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="667" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="668" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="669" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="670" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="671" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="672" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="673" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="674" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="675" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="676" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="677" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="678" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="679" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="680" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="681" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="682" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="683" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="684" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="685" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="686" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="687" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="688" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="689" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="690" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="691" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="692" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="693" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="694" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="695" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="696" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="697" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="698" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="699" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="700" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="701" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="702" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="703" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="704" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="705" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="706" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="707" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="708" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="709" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="710" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="711" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="712" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="713" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="714" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="715" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="716" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="717" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="718" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="719" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="720" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="721" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="722" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="723" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="724" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="725" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="726" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="727" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="728" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="729" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="730" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="731" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="732" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="733" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="734" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="735" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="736" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="737" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="738" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="739" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="740" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="741" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="742" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="743" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="744" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="745" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="746" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="747" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="748" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="749" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="750" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="751" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="752" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="753" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="754" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="755" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="756" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="757" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="758" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="759" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="760" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="761" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="762" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="763" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="764" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="765" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="766" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="767" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="768" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="769" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="770" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="771" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="772" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="773" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="774" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="775" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="776" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="777" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="778" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="779" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="780" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="781" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="782" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="783" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="784" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="785" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="786" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="787" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="788" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="789" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="790" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="791" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="792" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="793" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="794" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="795" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="796" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="797" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="798" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="799" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="800" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="801" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="802" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="803" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="804" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="805" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="806" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="807" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="808" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="809" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="810" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="811" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="812" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="813" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="814" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="815" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="816" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="817" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="818" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="819" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="820" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="821" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="822" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="823" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="824" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="825" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="826" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="827" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="828" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="829" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="830" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="831" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="832" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="833" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="834" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="835" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="836" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="837" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="838" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="839" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="840" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="841" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="842" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="843" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="844" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="845" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="846" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="847" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="848" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="849" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="850" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="851" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="852" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="853" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="854" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="855" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="856" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="857" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="858" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="859" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="860" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="861" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="862" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="863" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="864" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="865" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="866" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="867" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="868" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="869" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="870" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="871" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="872" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="873" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="874" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="875" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="876" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="877" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="878" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="879" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="880" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="881" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="882" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="883" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="884" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="885" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="886" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="887" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="888" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="889" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="890" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="891" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="892" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="893" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="894" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="895" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="896" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="897" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="898" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="899" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="900" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="901" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="902" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="903" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="904" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="905" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="906" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="907" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="908" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="909" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="910" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="911" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="912" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="913" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="914" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="915" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="916" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="917" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="918" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="919" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="920" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="921" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="922" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="923" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="924" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="925" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="926" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="927" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="928" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="929" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="930" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="931" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="932" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="933" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="934" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="935" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="936" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="937" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="938" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="939" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="940" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="941" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="942" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="943" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="944" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="945" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="946" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="947" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="948" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="949" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="950" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="951" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="952" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="953" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="954" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="955" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="956" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="957" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="958" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="959" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="960" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="961" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="962" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="963" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="964" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="965" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="966" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="967" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="968" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="969" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="970" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="971" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="972" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="973" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="974" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="975" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="976" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="977" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="978" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="979" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="980" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="981" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="982" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="983" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="984" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="195" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="227" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="228" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="229" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="232" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="233" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="275" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="276" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="277" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="278" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="291" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="293" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="294" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="295" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="303" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="304" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="305" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="306" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="307" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="308" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="309" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="310" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="311" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="312" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="317" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="318" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="319" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="320" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="321" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="322" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="323" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="324" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="325" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="329" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="330" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="331" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="332" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="334" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="335" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="336" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="337" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="338" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="339" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="340" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="341" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="342" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="343" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="344" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="345" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="346" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="347" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="348" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="350" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="358" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="359" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="360" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="361" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="362" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="363" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="364" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="365" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="366" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="367" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="368" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="369" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="370" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="371" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="372" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="373" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="374" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="375" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="376" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="377" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="378" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="379" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="380" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="381" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="383" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="384" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="385" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="386" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="387" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="388" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="389" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="390" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="391" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="392" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="393" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="394" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="395" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="396" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="397" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="398" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="399" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="400" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="401" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="402" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="403" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="404" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="405" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="406" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="407" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="408" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="409" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="410" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="411" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="412" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="413" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="414" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="415" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="416" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="417" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="418" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="419" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="420" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="421" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="422" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="423" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="424" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="425" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="426" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="427" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="428" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="429" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="430" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="431" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="432" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="433" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="434" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="435" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="436" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="437" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="438" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="439" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="440" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="441" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="442" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="443" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="444" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="445" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="446" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="447" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="448" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="449" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="450" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="451" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="452" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="453" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="454" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="455" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="456" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="457" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="458" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="459" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="460" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="461" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="462" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="463" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="464" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="465" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="466" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="467" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="468" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="469" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="470" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="471" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="472" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="473" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="474" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="475" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="476" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="477" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="478" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="480" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="481" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="482" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="483" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="484" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="485" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="486" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="487" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="488" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="489" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="490" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="491" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="492" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="493" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="494" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="495" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="496" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="497" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="498" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="499" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="500" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="501" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="502" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="503" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="504" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="505" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="506" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="507" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="508" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="509" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="510" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="511" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="512" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="513" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="514" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="515" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="516" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="517" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="518" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="519" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="520" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="521" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="522" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="523" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="524" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="525" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="526" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="527" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="528" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="529" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="530" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="531" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="532" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="533" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="534" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="535" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="536" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="537" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="538" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="539" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="540" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="541" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="542" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="543" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="544" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="545" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="546" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="547" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="548" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="549" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="550" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="551" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="552" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="553" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="554" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="555" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="556" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="557" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="558" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="559" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="560" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="561" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="562" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="563" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="564" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="565" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="566" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="567" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="568" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="569" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="570" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="571" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="572" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="573" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="574" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="575" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="576" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="577" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="578" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="579" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="580" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="581" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="582" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="583" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="584" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="585" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="586" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="587" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="588" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="589" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="590" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="591" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="592" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="593" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="594" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="595" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="596" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="597" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="598" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="599" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="600" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="601" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="602" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="603" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="604" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="605" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="606" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="607" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="608" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="609" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="610" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="611" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="612" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="613" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="614" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="615" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="616" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="617" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="618" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="619" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="620" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="621" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="622" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="623" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="624" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="625" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="626" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="627" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="628" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="629" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="630" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="631" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="632" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="633" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="634" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="635" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="636" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="637" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="638" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="639" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="640" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="641" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="642" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="643" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="644" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="645" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="646" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="647" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="648" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="649" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="650" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="651" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="652" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="653" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="654" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="655" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="656" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="657" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="658" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="659" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="660" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="661" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="662" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="663" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="664" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="665" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="666" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="667" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="668" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="669" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="670" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="671" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="672" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="673" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="674" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="675" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="676" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="677" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="678" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="679" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="680" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="681" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="682" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="683" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="684" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="685" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="686" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="687" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="688" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="689" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="690" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="691" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="692" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="693" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="694" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="695" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="696" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="697" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="698" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="699" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="700" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="701" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="702" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="703" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="704" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="705" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="706" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="707" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="708" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="709" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="710" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="711" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="712" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="713" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="714" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="715" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="716" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="717" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="718" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="719" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="720" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="721" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="722" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="723" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="724" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="725" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="726" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="727" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="728" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="729" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="730" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="731" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="732" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="733" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="734" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="735" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="736" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="737" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="738" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="739" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="740" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="741" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="742" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="743" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="744" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="745" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="746" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="747" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="748" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="749" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="750" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="751" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="752" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="753" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="754" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="755" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="756" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="757" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="758" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="759" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="760" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="761" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="762" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="763" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="764" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="765" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="766" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="767" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="768" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="769" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="770" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="771" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="772" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="773" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="774" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="775" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="776" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="777" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="778" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="779" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="780" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="781" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="782" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="783" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="784" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="785" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="786" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="787" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="788" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="789" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="790" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="791" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="792" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="793" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="794" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="795" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="796" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="797" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="798" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="799" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="800" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="801" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="802" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="803" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="804" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="805" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="806" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="807" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="808" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="809" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="810" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="811" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="812" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="813" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="814" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="815" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="816" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="817" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="818" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="819" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="820" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="821" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="822" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="823" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="824" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="825" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="826" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="827" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="828" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="829" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="830" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="831" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="832" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="833" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="834" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="835" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="836" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="837" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="838" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="839" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="840" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="841" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="842" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="843" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="844" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="845" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="846" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="847" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="848" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="849" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="850" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="851" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="852" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="853" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="854" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="855" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="856" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="857" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="858" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="859" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="860" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="861" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="862" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="863" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="864" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="865" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="866" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="867" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="868" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="869" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="870" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="871" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="872" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="873" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="874" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="875" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="876" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="877" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="878" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="879" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="880" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="881" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="882" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="883" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="884" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="885" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="886" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="887" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="888" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="889" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="890" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="891" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="892" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="893" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="894" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="895" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="896" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="897" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="898" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="899" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="900" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="901" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="902" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="903" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="904" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="905" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="906" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="907" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="908" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="909" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="910" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="911" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="912" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="913" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="914" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="915" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="916" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="917" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="918" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="919" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="920" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="921" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="922" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="923" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="924" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="925" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="926" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="927" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="928" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="929" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="930" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="931" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="932" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="933" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="934" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="935" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="936" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="937" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="938" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="939" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="940" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="941" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="942" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="943" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="944" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="945" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="946" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="947" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="948" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="949" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="950" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="951" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="952" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="953" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="954" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="955" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="956" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="957" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="958" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="959" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="960" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="961" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="962" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="963" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="964" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="965" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="966" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="967" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="968" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="969" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="970" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="971" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="972" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="973" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="974" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="975" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="976" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="977" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="978" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="979" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="980" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="981" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="982" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="983" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="984" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="985" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="986" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="991" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="0IyfwlA6iuEuaiYnZ0Ogkcr2bzdWNdksJE6ky3hKySSP7ddnwdaw0Fib8zGI4VWb6RaNYA+mszsOa3MNKK8jmQ==" saltValue="y4dbB0fRrV6/vEewMAdX9A==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
Still to fix the serch
</commit_message>
<xml_diff>
--- a/Position_surname.xlsx
+++ b/Position_surname.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\IMY220-D1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72CA2AE8-4790-4778-AA74-F749515B2905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC50B03-ABAC-4695-B2A9-C51EB997B750}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="149">
   <si>
     <t xml:space="preserve">Position_Surname: </t>
   </si>
@@ -1254,8 +1254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="A160" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B181" sqref="B181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1658,7 +1658,9 @@
       <c r="A62" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B62" s="36"/>
+      <c r="B62" s="36" t="s">
+        <v>148</v>
+      </c>
       <c r="C62" s="9">
         <v>1</v>
       </c>
@@ -1667,7 +1669,9 @@
       <c r="A63" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B63" s="36"/>
+      <c r="B63" s="36" t="s">
+        <v>148</v>
+      </c>
       <c r="C63" s="9">
         <v>1</v>
       </c>
@@ -1676,7 +1680,9 @@
       <c r="A64" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B64" s="36"/>
+      <c r="B64" s="36" t="s">
+        <v>148</v>
+      </c>
       <c r="C64" s="9">
         <v>1</v>
       </c>
@@ -1685,7 +1691,9 @@
       <c r="A65" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B65" s="36"/>
+      <c r="B65" s="36" t="s">
+        <v>148</v>
+      </c>
       <c r="C65" s="9">
         <v>1</v>
       </c>
@@ -1711,7 +1719,9 @@
       <c r="A69" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B69" s="36"/>
+      <c r="B69" s="36" t="s">
+        <v>148</v>
+      </c>
       <c r="C69" s="9">
         <v>1</v>
       </c>
@@ -1720,7 +1730,9 @@
       <c r="A70" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B70" s="36"/>
+      <c r="B70" s="36" t="s">
+        <v>148</v>
+      </c>
       <c r="C70" s="9">
         <v>1</v>
       </c>
@@ -2550,7 +2562,9 @@
       <c r="A172" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="B172" s="36"/>
+      <c r="B172" s="36" t="s">
+        <v>148</v>
+      </c>
       <c r="C172" s="9">
         <v>1</v>
       </c>
@@ -2559,7 +2573,9 @@
       <c r="A173" s="7" t="s">
         <v>135</v>
       </c>
-      <c r="B173" s="36"/>
+      <c r="B173" s="36" t="s">
+        <v>148</v>
+      </c>
       <c r="C173" s="9">
         <v>1</v>
       </c>
@@ -2568,7 +2584,9 @@
       <c r="A174" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="B174" s="36"/>
+      <c r="B174" s="36" t="s">
+        <v>148</v>
+      </c>
       <c r="C174" s="9">
         <v>1</v>
       </c>
@@ -2578,7 +2596,9 @@
       <c r="A175" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="B175" s="36"/>
+      <c r="B175" s="36" t="s">
+        <v>148</v>
+      </c>
       <c r="C175" s="9">
         <v>1</v>
       </c>
@@ -2588,7 +2608,9 @@
       <c r="A176" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="B176" s="36"/>
+      <c r="B176" s="36" t="s">
+        <v>148</v>
+      </c>
       <c r="C176" s="9">
         <v>2</v>
       </c>
@@ -2598,7 +2620,9 @@
       <c r="A177" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="B177" s="36"/>
+      <c r="B177" s="36" t="s">
+        <v>148</v>
+      </c>
       <c r="C177" s="9">
         <v>2</v>
       </c>
@@ -2607,7 +2631,9 @@
       <c r="A178" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B178" s="36"/>
+      <c r="B178" s="36" t="s">
+        <v>148</v>
+      </c>
       <c r="C178" s="9">
         <v>2</v>
       </c>
@@ -2616,7 +2642,9 @@
       <c r="A179" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="B179" s="36"/>
+      <c r="B179" s="36" t="s">
+        <v>148</v>
+      </c>
       <c r="C179" s="9">
         <v>2</v>
       </c>
@@ -2625,7 +2653,9 @@
       <c r="A180" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="B180" s="36"/>
+      <c r="B180" s="36" t="s">
+        <v>148</v>
+      </c>
       <c r="C180" s="9">
         <v>2</v>
       </c>
@@ -2634,7 +2664,9 @@
       <c r="A181" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="B181" s="36"/>
+      <c r="B181" s="36" t="s">
+        <v>148</v>
+      </c>
       <c r="C181" s="9">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Have to do the chech in out
</commit_message>
<xml_diff>
--- a/Position_surname.xlsx
+++ b/Position_surname.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\IMY220-D1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC50B03-ABAC-4695-B2A9-C51EB997B750}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C0C2DC-666A-4018-AB61-47936FE4E87A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,10 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="149">
-  <si>
-    <t xml:space="preserve">Position_Surname: </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="149">
   <si>
     <t>Yes/No</t>
   </si>
@@ -709,6 +706,9 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">47_Mokgothadi: </t>
   </si>
 </sst>
 </file>
@@ -1254,8 +1254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B181" sqref="B181"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1269,158 +1269,158 @@
   <sheetData>
     <row r="1" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="36" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" s="36"/>
     </row>
     <row r="16" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="36"/>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" s="36"/>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="36"/>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="36"/>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" s="36"/>
     </row>
     <row r="23" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" s="36"/>
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B24" s="36"/>
     </row>
     <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B25" s="36"/>
     </row>
     <row r="26" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B26" s="36"/>
     </row>
     <row r="27" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B27" s="36"/>
     </row>
     <row r="28" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B30" s="8"/>
     </row>
     <row r="31" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B31" s="8"/>
     </row>
     <row r="32" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B32" s="8"/>
     </row>
@@ -1431,13 +1431,13 @@
     <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="str">
         <f>A1</f>
-        <v xml:space="preserve">Position_Surname: </v>
+        <v xml:space="preserve">47_Mokgothadi: </v>
       </c>
       <c r="B34" s="7"/>
     </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
@@ -1445,15 +1445,15 @@
     <row r="36" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B38" s="36" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C38" s="9">
         <v>1</v>
@@ -1461,10 +1461,10 @@
     </row>
     <row r="39" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B39" s="36" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C39" s="9">
         <v>1</v>
@@ -1472,10 +1472,10 @@
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B40" s="36" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C40" s="9">
         <v>1</v>
@@ -1483,10 +1483,10 @@
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B41" s="36" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C41" s="9">
         <v>1</v>
@@ -1499,7 +1499,7 @@
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B43" s="36"/>
       <c r="C43" s="13">
@@ -1509,15 +1509,15 @@
     <row r="44" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B46" s="36" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C46" s="9">
         <v>1</v>
@@ -1525,10 +1525,10 @@
     </row>
     <row r="47" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B47" s="36" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C47" s="9">
         <v>1</v>
@@ -1536,10 +1536,10 @@
     </row>
     <row r="48" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B48" s="36" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C48" s="9">
         <v>1</v>
@@ -1547,10 +1547,10 @@
     </row>
     <row r="49" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B49" s="36" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C49" s="9">
         <v>1</v>
@@ -1558,10 +1558,10 @@
     </row>
     <row r="50" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B50" s="36" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C50" s="9">
         <v>1</v>
@@ -1569,10 +1569,10 @@
     </row>
     <row r="51" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B51" s="36" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C51" s="9">
         <v>1</v>
@@ -1580,10 +1580,10 @@
     </row>
     <row r="52" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B52" s="36" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C52" s="9">
         <v>1</v>
@@ -1591,10 +1591,10 @@
     </row>
     <row r="53" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B53" s="36" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C53" s="9">
         <v>1</v>
@@ -1602,7 +1602,7 @@
     </row>
     <row r="54" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B54" s="36"/>
       <c r="C54" s="9">
@@ -1616,10 +1616,10 @@
     </row>
     <row r="56" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B56" s="36" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C56" s="13">
         <v>2</v>
@@ -1627,9 +1627,11 @@
     </row>
     <row r="57" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="B57" s="36"/>
+        <v>45</v>
+      </c>
+      <c r="B57" s="36" t="s">
+        <v>147</v>
+      </c>
       <c r="C57" s="9">
         <v>3</v>
       </c>
@@ -1637,17 +1639,17 @@
     <row r="58" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="59" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B61" s="36"/>
       <c r="C61" s="9">
@@ -1656,10 +1658,10 @@
     </row>
     <row r="62" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B62" s="36" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C62" s="9">
         <v>1</v>
@@ -1667,10 +1669,10 @@
     </row>
     <row r="63" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B63" s="36" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C63" s="9">
         <v>1</v>
@@ -1678,10 +1680,10 @@
     </row>
     <row r="64" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B64" s="36" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C64" s="9">
         <v>1</v>
@@ -1689,10 +1691,10 @@
     </row>
     <row r="65" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B65" s="36" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C65" s="9">
         <v>1</v>
@@ -1700,7 +1702,7 @@
     </row>
     <row r="66" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B66" s="36"/>
       <c r="C66" s="9">
@@ -1712,15 +1714,15 @@
     </row>
     <row r="68" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B69" s="36" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C69" s="9">
         <v>1</v>
@@ -1728,10 +1730,10 @@
     </row>
     <row r="70" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B70" s="36" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C70" s="9">
         <v>1</v>
@@ -1739,7 +1741,7 @@
     </row>
     <row r="71" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B71" s="36"/>
       <c r="C71" s="9">
@@ -1748,25 +1750,29 @@
     </row>
     <row r="72" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B72" s="36"/>
+        <v>58</v>
+      </c>
+      <c r="B72" s="36" t="s">
+        <v>147</v>
+      </c>
       <c r="C72" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="B73" s="36"/>
+        <v>59</v>
+      </c>
+      <c r="B73" s="36" t="s">
+        <v>147</v>
+      </c>
       <c r="C73" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B74" s="36"/>
       <c r="C74" s="9">
@@ -1776,30 +1782,34 @@
     <row r="75" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="76" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B77" s="36"/>
+        <v>62</v>
+      </c>
+      <c r="B77" s="36" t="s">
+        <v>147</v>
+      </c>
       <c r="C77" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B78" s="36"/>
+        <v>63</v>
+      </c>
+      <c r="B78" s="36" t="s">
+        <v>147</v>
+      </c>
       <c r="C78" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B79" s="36"/>
       <c r="C79" s="9">
@@ -1808,7 +1818,7 @@
     </row>
     <row r="80" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B80" s="36"/>
       <c r="C80" s="13">
@@ -1822,27 +1832,33 @@
     </row>
     <row r="82" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="B82" s="36"/>
+        <v>66</v>
+      </c>
+      <c r="B82" s="36" t="s">
+        <v>147</v>
+      </c>
       <c r="C82" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B83" s="36"/>
+        <v>67</v>
+      </c>
+      <c r="B83" s="36" t="s">
+        <v>147</v>
+      </c>
       <c r="C83" s="9">
         <v>3</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="B84" s="36"/>
+        <v>68</v>
+      </c>
+      <c r="B84" s="36" t="s">
+        <v>147</v>
+      </c>
       <c r="C84" s="9">
         <v>2</v>
       </c>
@@ -1854,21 +1870,23 @@
     </row>
     <row r="86" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B87" s="36"/>
+        <v>70</v>
+      </c>
+      <c r="B87" s="36" t="s">
+        <v>147</v>
+      </c>
       <c r="C87" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B88" s="36"/>
       <c r="C88" s="13">
@@ -1877,7 +1895,7 @@
     </row>
     <row r="89" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B89" s="36"/>
       <c r="C89" s="13">
@@ -1886,7 +1904,7 @@
     </row>
     <row r="90" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B90" s="36"/>
       <c r="C90" s="13">
@@ -1895,7 +1913,7 @@
     </row>
     <row r="91" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B91" s="36"/>
       <c r="C91" s="13">
@@ -1909,7 +1927,7 @@
     </row>
     <row r="93" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B93" s="36"/>
       <c r="C93" s="13">
@@ -1918,7 +1936,7 @@
     </row>
     <row r="94" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B94" s="36"/>
       <c r="C94" s="13">
@@ -1932,12 +1950,12 @@
     </row>
     <row r="96" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B97" s="36"/>
       <c r="C97" s="13">
@@ -1946,7 +1964,7 @@
     </row>
     <row r="98" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B98" s="36"/>
       <c r="C98" s="13">
@@ -1955,7 +1973,7 @@
     </row>
     <row r="99" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B99" s="36"/>
       <c r="C99" s="13">
@@ -1964,7 +1982,7 @@
     </row>
     <row r="100" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B100" s="36"/>
       <c r="C100" s="13">
@@ -1973,7 +1991,7 @@
     </row>
     <row r="101" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B101" s="36"/>
       <c r="C101" s="9">
@@ -1986,32 +2004,36 @@
     </row>
     <row r="103" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B103" s="11"/>
       <c r="C103" s="7"/>
     </row>
     <row r="104" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="B104" s="36"/>
+        <v>84</v>
+      </c>
+      <c r="B104" s="36" t="s">
+        <v>147</v>
+      </c>
       <c r="C104" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="B105" s="36"/>
+        <v>85</v>
+      </c>
+      <c r="B105" s="36" t="s">
+        <v>147</v>
+      </c>
       <c r="C105" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B106" s="36"/>
       <c r="C106" s="13">
@@ -2025,7 +2047,7 @@
     </row>
     <row r="108" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B108" s="36"/>
       <c r="C108" s="13">
@@ -2038,34 +2060,40 @@
     </row>
     <row r="110" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B110" s="11"/>
       <c r="C110" s="7"/>
     </row>
     <row r="111" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="B111" s="36"/>
+        <v>89</v>
+      </c>
+      <c r="B111" s="36" t="s">
+        <v>147</v>
+      </c>
       <c r="C111" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="B112" s="36"/>
+        <v>90</v>
+      </c>
+      <c r="B112" s="36" t="s">
+        <v>147</v>
+      </c>
       <c r="C112" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="113" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="B113" s="36"/>
+        <v>91</v>
+      </c>
+      <c r="B113" s="36" t="s">
+        <v>147</v>
+      </c>
       <c r="C113" s="13">
         <v>1</v>
       </c>
@@ -2077,7 +2105,7 @@
     </row>
     <row r="115" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="16" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B115" s="36"/>
       <c r="C115" s="13">
@@ -2086,9 +2114,11 @@
     </row>
     <row r="116" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A116" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="B116" s="36"/>
+        <v>93</v>
+      </c>
+      <c r="B116" s="36" t="s">
+        <v>147</v>
+      </c>
       <c r="C116" s="13">
         <v>2</v>
       </c>
@@ -2100,21 +2130,21 @@
     </row>
     <row r="118" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B118" s="7"/>
       <c r="C118" s="7"/>
     </row>
     <row r="119" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A119" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B119" s="11"/>
       <c r="C119" s="7"/>
     </row>
     <row r="120" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A120" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B120" s="36"/>
       <c r="C120" s="9">
@@ -2123,7 +2153,7 @@
     </row>
     <row r="121" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B121" s="36"/>
       <c r="C121" s="9">
@@ -2132,7 +2162,7 @@
     </row>
     <row r="122" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A122" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B122" s="36"/>
       <c r="C122" s="9">
@@ -2141,7 +2171,7 @@
     </row>
     <row r="123" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B123" s="36"/>
       <c r="C123" s="9">
@@ -2150,7 +2180,7 @@
     </row>
     <row r="124" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B124" s="36"/>
       <c r="C124" s="9">
@@ -2164,7 +2194,7 @@
     </row>
     <row r="126" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B126" s="36"/>
       <c r="C126" s="9">
@@ -2181,7 +2211,7 @@
     </row>
     <row r="128" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B128" s="8"/>
       <c r="C128" s="9"/>
@@ -2192,7 +2222,7 @@
     </row>
     <row r="129" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B129" s="7"/>
       <c r="C129" s="7"/>
@@ -2249,7 +2279,7 @@
     <row r="135" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="str">
         <f>A1</f>
-        <v xml:space="preserve">Position_Surname: </v>
+        <v xml:space="preserve">47_Mokgothadi: </v>
       </c>
       <c r="B135" s="7"/>
       <c r="C135" s="7"/>
@@ -2260,7 +2290,7 @@
     </row>
     <row r="136" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B136" s="8"/>
       <c r="C136" s="9"/>
@@ -2271,14 +2301,14 @@
     </row>
     <row r="138" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B138" s="7"/>
       <c r="C138" s="7"/>
     </row>
     <row r="139" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B139" s="36"/>
       <c r="C139" s="9">
@@ -2287,7 +2317,7 @@
     </row>
     <row r="140" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B140" s="36"/>
       <c r="C140" s="9">
@@ -2296,9 +2326,11 @@
     </row>
     <row r="141" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A141" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="B141" s="37"/>
+        <v>108</v>
+      </c>
+      <c r="B141" s="37" t="s">
+        <v>147</v>
+      </c>
       <c r="C141" s="24">
         <v>3</v>
       </c>
@@ -2328,7 +2360,7 @@
     </row>
     <row r="142" spans="1:26" ht="135" x14ac:dyDescent="0.25">
       <c r="A142" s="26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B142" s="11"/>
       <c r="C142" s="7"/>
@@ -2340,7 +2372,7 @@
     </row>
     <row r="144" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B144" s="36"/>
       <c r="C144" s="13">
@@ -2353,14 +2385,14 @@
     </row>
     <row r="146" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A146" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B146" s="11"/>
       <c r="C146" s="7"/>
     </row>
     <row r="147" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A147" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B147" s="36"/>
       <c r="C147" s="9">
@@ -2369,7 +2401,7 @@
     </row>
     <row r="148" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B148" s="36"/>
       <c r="C148" s="9">
@@ -2378,7 +2410,7 @@
     </row>
     <row r="149" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B149" s="36"/>
       <c r="C149" s="9">
@@ -2387,7 +2419,7 @@
     </row>
     <row r="150" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B150" s="36"/>
       <c r="C150" s="9">
@@ -2396,7 +2428,7 @@
     </row>
     <row r="151" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B151" s="36"/>
       <c r="C151" s="9">
@@ -2405,7 +2437,7 @@
     </row>
     <row r="152" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B152" s="36"/>
       <c r="C152" s="9">
@@ -2414,7 +2446,7 @@
     </row>
     <row r="153" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B153" s="36"/>
       <c r="C153" s="9">
@@ -2423,7 +2455,7 @@
     </row>
     <row r="154" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B154" s="36"/>
       <c r="C154" s="9">
@@ -2432,7 +2464,7 @@
     </row>
     <row r="155" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B155" s="36"/>
       <c r="C155" s="9">
@@ -2441,7 +2473,7 @@
     </row>
     <row r="156" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B156" s="36"/>
       <c r="C156" s="9">
@@ -2450,7 +2482,7 @@
     </row>
     <row r="157" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="28" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B157" s="36"/>
       <c r="C157" s="13">
@@ -2464,7 +2496,7 @@
     </row>
     <row r="159" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="28" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B159" s="36"/>
       <c r="C159" s="9">
@@ -2477,14 +2509,14 @@
     </row>
     <row r="161" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B161" s="7"/>
       <c r="C161" s="7"/>
     </row>
     <row r="162" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B162" s="8"/>
       <c r="C162" s="9">
@@ -2497,14 +2529,14 @@
     </row>
     <row r="164" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B164" s="7"/>
       <c r="C164" s="7"/>
     </row>
     <row r="165" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B165" s="36"/>
       <c r="C165" s="9">
@@ -2513,7 +2545,7 @@
     </row>
     <row r="166" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B166" s="36"/>
       <c r="C166" s="9">
@@ -2522,7 +2554,7 @@
     </row>
     <row r="167" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B167" s="36"/>
       <c r="C167" s="9">
@@ -2531,7 +2563,7 @@
     </row>
     <row r="168" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B168" s="36"/>
       <c r="C168" s="9">
@@ -2540,7 +2572,7 @@
     </row>
     <row r="169" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B169" s="36"/>
       <c r="C169" s="9">
@@ -2553,40 +2585,34 @@
     </row>
     <row r="171" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A171" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B171" s="7"/>
       <c r="C171" s="7"/>
     </row>
     <row r="172" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A172" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="B172" s="36" t="s">
-        <v>148</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="B172" s="36"/>
       <c r="C172" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="173" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A173" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="B173" s="36" t="s">
-        <v>148</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="B173" s="36"/>
       <c r="C173" s="9">
         <v>1</v>
       </c>
     </row>
     <row r="174" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A174" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="B174" s="36" t="s">
-        <v>148</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="B174" s="36"/>
       <c r="C174" s="9">
         <v>1</v>
       </c>
@@ -2594,11 +2620,9 @@
     </row>
     <row r="175" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="B175" s="36" t="s">
-        <v>148</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="B175" s="36"/>
       <c r="C175" s="9">
         <v>1</v>
       </c>
@@ -2606,11 +2630,9 @@
     </row>
     <row r="176" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="B176" s="36" t="s">
-        <v>148</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="B176" s="36"/>
       <c r="C176" s="9">
         <v>2</v>
       </c>
@@ -2618,55 +2640,45 @@
     </row>
     <row r="177" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="B177" s="36" t="s">
-        <v>148</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="B177" s="36"/>
       <c r="C177" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="178" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="B178" s="36" t="s">
-        <v>148</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="B178" s="36"/>
       <c r="C178" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="179" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="B179" s="36" t="s">
-        <v>148</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="B179" s="36"/>
       <c r="C179" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="180" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="B180" s="36" t="s">
-        <v>148</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="B180" s="36"/>
       <c r="C180" s="9">
         <v>2</v>
       </c>
     </row>
     <row r="181" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="B181" s="36" t="s">
-        <v>148</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="B181" s="36"/>
       <c r="C181" s="9">
         <v>2</v>
       </c>
@@ -2676,13 +2688,13 @@
     </row>
     <row r="183" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C183" s="7"/>
     </row>
     <row r="184" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B184" s="36"/>
       <c r="C184" s="30">
@@ -2694,14 +2706,14 @@
     </row>
     <row r="186" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B186" s="8"/>
       <c r="C186" s="9"/>
     </row>
     <row r="187" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C187" s="7"/>
     </row>
@@ -2727,7 +2739,7 @@
     </row>
     <row r="192" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A192" s="33" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B192" s="34"/>
       <c r="C192" s="33">
@@ -2737,7 +2749,7 @@
     </row>
     <row r="193" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="35" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B193" s="34"/>
       <c r="C193" s="33">
@@ -2747,7 +2759,7 @@
     </row>
     <row r="194" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A194" s="33" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B194" s="34"/>
       <c r="C194" s="33">

</xml_diff>